<commit_message>
initial geoprofile processing from general QUDT UoM & QKs
</commit_message>
<xml_diff>
--- a/resources/GSQ_UNITS_OF_MEASURE.xlsx
+++ b/resources/GSQ_UNITS_OF_MEASURE.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/gsq/qudt-geo-profile-ont/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/qudt-geo-profile-ont/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0428ABC-9155-384F-AAC6-5152F3834009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15788B08-9422-1741-93BE-409AA251AF27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1700" yWindow="-21140" windowWidth="38400" windowHeight="21140"/>
+    <workbookView xWindow="1920" yWindow="460" windowWidth="31680" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GSQ_UNITS_OF_MEASURE" sheetId="1" r:id="rId1"/>
+    <sheet name="Consolidated Lists" sheetId="2" r:id="rId2"/>
+    <sheet name="Quantity Kinds" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="386">
   <si>
     <t>Additive Quantity</t>
   </si>
@@ -1202,12 +1204,362 @@
   <si>
     <t>Count</t>
   </si>
+  <si>
+    <t>unit:GAL_US</t>
+  </si>
+  <si>
+    <r>
+      <t>unit:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>GAL_IMP</t>
+    </r>
+  </si>
+  <si>
+    <t>From Results Vocab</t>
+  </si>
+  <si>
+    <t>rslt:api-gravity</t>
+  </si>
+  <si>
+    <t>rslt:area</t>
+  </si>
+  <si>
+    <t>rslt:capacitance</t>
+  </si>
+  <si>
+    <t>rslt:casing-weight</t>
+  </si>
+  <si>
+    <t>rslt:colour</t>
+  </si>
+  <si>
+    <t>rslt:composition</t>
+  </si>
+  <si>
+    <t>rslt:compressibility</t>
+  </si>
+  <si>
+    <t>rslt:compressive-strength</t>
+  </si>
+  <si>
+    <t>rslt:concentration</t>
+  </si>
+  <si>
+    <t>rslt:conductivity</t>
+  </si>
+  <si>
+    <t>rslt:cost</t>
+  </si>
+  <si>
+    <t>rslt:count</t>
+  </si>
+  <si>
+    <t>rslt:data</t>
+  </si>
+  <si>
+    <t>rslt:density</t>
+  </si>
+  <si>
+    <t>rslt:descriptive</t>
+  </si>
+  <si>
+    <t>rslt:distance</t>
+  </si>
+  <si>
+    <t>rslt:dog-leg-severity</t>
+  </si>
+  <si>
+    <t>rslt:drill-rate</t>
+  </si>
+  <si>
+    <t>rslt:electric-charge</t>
+  </si>
+  <si>
+    <t>rslt:electric-current</t>
+  </si>
+  <si>
+    <t>rslt:energy</t>
+  </si>
+  <si>
+    <t>rslt:energy-density</t>
+  </si>
+  <si>
+    <t>rslt:flow-rate</t>
+  </si>
+  <si>
+    <t>rslt:fluid-density</t>
+  </si>
+  <si>
+    <t>rslt:force</t>
+  </si>
+  <si>
+    <t>rslt:frequency</t>
+  </si>
+  <si>
+    <t>rslt:gas-content</t>
+  </si>
+  <si>
+    <t>rslt:grain-shape</t>
+  </si>
+  <si>
+    <t>rslt:grain-size</t>
+  </si>
+  <si>
+    <t>rslt:heat</t>
+  </si>
+  <si>
+    <t>rslt:illuminance</t>
+  </si>
+  <si>
+    <t>rslt:inductance</t>
+  </si>
+  <si>
+    <t>rslt:length</t>
+  </si>
+  <si>
+    <t>rslt:luminous-flux</t>
+  </si>
+  <si>
+    <t>rslt:luminous-intensity</t>
+  </si>
+  <si>
+    <t>rslt:magnetic-flux</t>
+  </si>
+  <si>
+    <t>rslt:magnetic-flux-density</t>
+  </si>
+  <si>
+    <t>rslt:mass</t>
+  </si>
+  <si>
+    <t>rslt:measured-depth</t>
+  </si>
+  <si>
+    <t>rslt:oil-quality</t>
+  </si>
+  <si>
+    <t>rslt:permeability</t>
+  </si>
+  <si>
+    <t>rslt:porosity</t>
+  </si>
+  <si>
+    <t>rslt:power</t>
+  </si>
+  <si>
+    <t>rslt:pressure</t>
+  </si>
+  <si>
+    <t>rslt:radioactivity</t>
+  </si>
+  <si>
+    <t>rslt:resitivity</t>
+  </si>
+  <si>
+    <t>rslt:rotation</t>
+  </si>
+  <si>
+    <t>rslt:saturation</t>
+  </si>
+  <si>
+    <t>rslt:shear-strength</t>
+  </si>
+  <si>
+    <t>rslt:sorting</t>
+  </si>
+  <si>
+    <t>rslt:spacing</t>
+  </si>
+  <si>
+    <t>rslt:sphericity</t>
+  </si>
+  <si>
+    <t>rslt:stiffness</t>
+  </si>
+  <si>
+    <t>rslt:strain</t>
+  </si>
+  <si>
+    <t>rslt:stress</t>
+  </si>
+  <si>
+    <t>rslt:temperature</t>
+  </si>
+  <si>
+    <t>rslt:tensile-strength</t>
+  </si>
+  <si>
+    <t>rslt:time</t>
+  </si>
+  <si>
+    <t>rslt:true-vertical-depth</t>
+  </si>
+  <si>
+    <t>rslt:velocity</t>
+  </si>
+  <si>
+    <t>rslt:viscosity</t>
+  </si>
+  <si>
+    <t>rslt:voltage</t>
+  </si>
+  <si>
+    <t>rslt:volume</t>
+  </si>
+  <si>
+    <t>rslt:wavelength</t>
+  </si>
+  <si>
+    <t>rslt:weight</t>
+  </si>
+  <si>
+    <t>rslt:weight-on-bit</t>
+  </si>
+  <si>
+    <t>rslt:work</t>
+  </si>
+  <si>
+    <t>rslt:yield-point</t>
+  </si>
+  <si>
+    <t>QUDT</t>
+  </si>
+  <si>
+    <t>quantitykind:Area</t>
+  </si>
+  <si>
+    <t>quantitykind:Capacitance</t>
+  </si>
+  <si>
+    <t>quantitykind:Compressibility</t>
+  </si>
+  <si>
+    <t>quantitykind:Concentration</t>
+  </si>
+  <si>
+    <t>quantitykind:Conductivity</t>
+  </si>
+  <si>
+    <t>quantitykind:Density</t>
+  </si>
+  <si>
+    <t>quantitykind:Distance</t>
+  </si>
+  <si>
+    <t>quantitykind:ElectricCharge</t>
+  </si>
+  <si>
+    <t>quantitykind:ElectricCurrent</t>
+  </si>
+  <si>
+    <t>quantitykind:Energy</t>
+  </si>
+  <si>
+    <t>quantitykind:EnergyDensity</t>
+  </si>
+  <si>
+    <t>quantitykind:VolumeFlowRate</t>
+  </si>
+  <si>
+    <t>quantitykind:Force</t>
+  </si>
+  <si>
+    <t>quantitykind:Frequency</t>
+  </si>
+  <si>
+    <t>quantitykind:HeatFlowRate</t>
+  </si>
+  <si>
+    <t>quantitykind:Illuminance</t>
+  </si>
+  <si>
+    <t>quantitykind:Inductance</t>
+  </si>
+  <si>
+    <t>quantitykind:Length</t>
+  </si>
+  <si>
+    <t>quantitykind:LuminousFlux</t>
+  </si>
+  <si>
+    <t>quantitykind:LuminousFluxPerArea
+quantitykind:LuminousIntensity</t>
+  </si>
+  <si>
+    <t>quantitykind:MagneticFlux</t>
+  </si>
+  <si>
+    <t>quantitykind:MagneticFluxDensity</t>
+  </si>
+  <si>
+    <t>quantitykind:Mass</t>
+  </si>
+  <si>
+    <t>quantitykind:Permeability</t>
+  </si>
+  <si>
+    <t>quantitykind:Power</t>
+  </si>
+  <si>
+    <t>quantitykind:Pressure</t>
+  </si>
+  <si>
+    <t>quantitykind:Radiosity?</t>
+  </si>
+  <si>
+    <t>quantitykind:Resistivity</t>
+  </si>
+  <si>
+    <t>quantitykind:ShearModulus?</t>
+  </si>
+  <si>
+    <t>quantitykind:ShearStrain?</t>
+  </si>
+  <si>
+    <t>quantitykind:ShearStress?</t>
+  </si>
+  <si>
+    <t>quantitykind:Temperature</t>
+  </si>
+  <si>
+    <t>quantitykind:Time</t>
+  </si>
+  <si>
+    <t>quantitykind:Velocity</t>
+  </si>
+  <si>
+    <t>quantitykind:Viscosity</t>
+  </si>
+  <si>
+    <t>quantitykind:Voltage</t>
+  </si>
+  <si>
+    <t>quantitykind:Volume</t>
+  </si>
+  <si>
+    <t>inv. Freq?</t>
+  </si>
+  <si>
+    <t>quantitykind:Weight</t>
+  </si>
+  <si>
+    <t>quantitykind:Work</t>
+  </si>
+  <si>
+    <t>quantitykind:LuminousIntensity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1352,6 +1704,14 @@
       <sz val="12"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1651,7 +2011,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1694,14 +2054,23 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1735,6 +2104,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2054,11 +2424,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="J207" sqref="J207"/>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4278,4 +4648,1434 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B21C88-1478-FB4D-A0EF-DE8427252580}">
+  <dimension ref="A1:J215"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" t="s">
+        <v>351</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" t="s">
+        <v>352</v>
+      </c>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" t="s">
+        <v>353</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" t="s">
+        <v>354</v>
+      </c>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" t="s">
+        <v>355</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" t="s">
+        <v>357</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D14" t="s">
+        <v>358</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D15" t="s">
+        <v>359</v>
+      </c>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" t="s">
+        <v>360</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D17" t="s">
+        <v>361</v>
+      </c>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D18" t="s">
+        <v>362</v>
+      </c>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D19" t="s">
+        <v>363</v>
+      </c>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D21" t="s">
+        <v>365</v>
+      </c>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D22" t="s">
+        <v>366</v>
+      </c>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D23" t="s">
+        <v>367</v>
+      </c>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D24" t="s">
+        <v>368</v>
+      </c>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D25" t="s">
+        <v>369</v>
+      </c>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D26" t="s">
+        <v>370</v>
+      </c>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>273</v>
+      </c>
+      <c r="D27" t="s">
+        <v>371</v>
+      </c>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D28" t="s">
+        <v>372</v>
+      </c>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D29" t="s">
+        <v>373</v>
+      </c>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D30" t="s">
+        <v>374</v>
+      </c>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D31" t="s">
+        <v>375</v>
+      </c>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D32" t="s">
+        <v>376</v>
+      </c>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D33" t="s">
+        <v>377</v>
+      </c>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D34" t="s">
+        <v>378</v>
+      </c>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D35" t="s">
+        <v>379</v>
+      </c>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D36" t="s">
+        <v>380</v>
+      </c>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D37" t="s">
+        <v>381</v>
+      </c>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D38" t="s">
+        <v>356</v>
+      </c>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D39" t="s">
+        <v>383</v>
+      </c>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D40" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D40">
+    <sortCondition ref="D2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAC2D2E-36D4-134F-A9AC-823DD4404679}">
+  <dimension ref="A1:C69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>285</v>
+      </c>
+      <c r="B11" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B15" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B20" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>295</v>
+      </c>
+      <c r="B21" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>296</v>
+      </c>
+      <c r="B22" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>298</v>
+      </c>
+      <c r="B24" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>299</v>
+      </c>
+      <c r="B25" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>300</v>
+      </c>
+      <c r="B26" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>301</v>
+      </c>
+      <c r="B27" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>305</v>
+      </c>
+      <c r="B31" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>306</v>
+      </c>
+      <c r="B32" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>307</v>
+      </c>
+      <c r="B33" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>308</v>
+      </c>
+      <c r="B34" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>309</v>
+      </c>
+      <c r="B35" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>310</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>311</v>
+      </c>
+      <c r="B37" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>312</v>
+      </c>
+      <c r="B38" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>313</v>
+      </c>
+      <c r="B39" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>316</v>
+      </c>
+      <c r="B42" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>318</v>
+      </c>
+      <c r="B44" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>319</v>
+      </c>
+      <c r="B45" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>320</v>
+      </c>
+      <c r="B46" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>321</v>
+      </c>
+      <c r="B47" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>324</v>
+      </c>
+      <c r="B50" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>329</v>
+      </c>
+      <c r="B55" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>330</v>
+      </c>
+      <c r="B56" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>331</v>
+      </c>
+      <c r="B57" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>333</v>
+      </c>
+      <c r="B59" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>335</v>
+      </c>
+      <c r="B61" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>336</v>
+      </c>
+      <c r="B62" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>337</v>
+      </c>
+      <c r="B63" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>338</v>
+      </c>
+      <c r="B64" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>339</v>
+      </c>
+      <c r="C65" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>340</v>
+      </c>
+      <c r="B66" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>342</v>
+      </c>
+      <c r="B68" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>343</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>